<commit_message>
Reformatetd DataScraperModel to an actual class
</commit_message>
<xml_diff>
--- a/data.xlsx
+++ b/data.xlsx
@@ -889,27 +889,27 @@
       </c>
       <c r="L6" s="1" t="inlineStr">
         <is>
-          <t>(816) 690-3177</t>
+          <t>(252) 232-3724</t>
         </is>
       </c>
       <c r="M6" s="1" t="inlineStr">
         <is>
-          <t>(816) 206-1455</t>
+          <t>(757) 424-0364</t>
         </is>
       </c>
       <c r="N6" s="1" t="inlineStr">
         <is>
-          <t>(816) 690-6956</t>
+          <t>(757) 424-1089</t>
         </is>
       </c>
       <c r="O6" s="1" t="inlineStr">
         <is>
-          <t>(816) 697-2151</t>
+          <t>(757) 482-3605</t>
         </is>
       </c>
       <c r="P6" s="1" t="inlineStr">
         <is>
-          <t>(816) 267-0195</t>
+          <t>(757) 560-6109</t>
         </is>
       </c>
     </row>
@@ -967,27 +967,27 @@
       </c>
       <c r="L7" s="1" t="inlineStr">
         <is>
-          <t>(913) 469-5942</t>
+          <t>(407) 344-9360</t>
         </is>
       </c>
       <c r="M7" s="1" t="inlineStr">
         <is>
-          <t>(636) 456-3715</t>
+          <t>(919) 402-4322</t>
         </is>
       </c>
       <c r="N7" s="1" t="inlineStr">
         <is>
-          <t>(913) 541-3340</t>
+          <t>(434) 791-2763</t>
         </is>
       </c>
       <c r="O7" s="1" t="inlineStr">
         <is>
-          <t>(913) 469-0000</t>
+          <t>(336) 602-2970</t>
         </is>
       </c>
       <c r="P7" s="1" t="inlineStr">
         <is>
-          <t>(469) 594-2000</t>
+          <t>(919) 926-0149</t>
         </is>
       </c>
     </row>
@@ -1201,27 +1201,27 @@
       </c>
       <c r="L10" s="1" t="inlineStr">
         <is>
-          <t>(660) 525-9956</t>
+          <t>(321) 200-7555</t>
         </is>
       </c>
       <c r="M10" s="1" t="inlineStr">
         <is>
-          <t>(660) 890-2757</t>
+          <t>(904) 460-7673</t>
         </is>
       </c>
       <c r="N10" s="1" t="inlineStr">
         <is>
-          <t>(660) 525-9570</t>
+          <t>(904) 683-3096</t>
         </is>
       </c>
       <c r="O10" s="1" t="inlineStr">
         <is>
-          <t>(505) 771-3496</t>
+          <t>(904) 388-9866</t>
         </is>
       </c>
       <c r="P10" s="1" t="inlineStr">
         <is>
-          <t>(660) 525-9032</t>
+          <t>(904) 683-8680</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Added Client Addition to SQL Database
</commit_message>
<xml_diff>
--- a/data.xlsx
+++ b/data.xlsx
@@ -464,7 +464,7 @@
   <dimension ref="A1:AH12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H4" sqref="H4"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="14.4"/>
@@ -572,12 +572,12 @@
     <row r="2">
       <c r="A2" s="2" t="inlineStr">
         <is>
-          <t>Arthur</t>
+          <t>Ced</t>
         </is>
       </c>
       <c r="B2" s="2" t="inlineStr">
         <is>
-          <t>Manzano</t>
+          <t>David</t>
         </is>
       </c>
       <c r="C2" s="2" t="inlineStr">
@@ -621,7 +621,11 @@
           <t>Saint Louis</t>
         </is>
       </c>
-      <c r="L2" s="1" t="n"/>
+      <c r="L2" s="1" t="inlineStr">
+        <is>
+          <t>(702) 885-5544</t>
+        </is>
+      </c>
       <c r="M2" s="1" t="n"/>
       <c r="N2" s="1" t="n"/>
       <c r="O2" s="1" t="n"/>

</xml_diff>